<commit_message>
commit de todo la cual salio la version final para agosto julio y junio 2022
</commit_message>
<xml_diff>
--- a/txt generated files/planillas que se necesitan para generar el txt/DATOS PERSONALES_TXT.xlsx
+++ b/txt generated files/planillas que se necesitan para generar el txt/DATOS PERSONALES_TXT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juanj\OneDrive\Documentos\txtgenerator\txtgenerator\txt generated files\planillas que se necesitan para generar el txt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A7D373-6C76-473E-ABCE-7A4F950E7BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FD3383-D677-4748-BDFF-CF074C41BDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="657">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="661">
   <si>
     <t>name</t>
   </si>
@@ -1996,6 +1996,18 @@
   </si>
   <si>
     <t>BASUALDO 2237, CABA</t>
+  </si>
+  <si>
+    <t>SEGOVIA JUAN JOSE</t>
+  </si>
+  <si>
+    <t>PRIETO 660 , ADROGUE</t>
+  </si>
+  <si>
+    <t>FLORELLI ELVIRA SUSANA</t>
+  </si>
+  <si>
+    <t>CUENCA 3345 6TO 32</t>
   </si>
 </sst>
 </file>
@@ -2354,10 +2366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H336"/>
+  <dimension ref="A1:H338"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H336"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2411,7 +2423,7 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>2234893429</v>
       </c>
       <c r="F2" s="2">
@@ -2437,7 +2449,7 @@
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>2234916476</v>
       </c>
       <c r="F3" s="2">
@@ -2463,7 +2475,7 @@
       <c r="D4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>2234727002</v>
       </c>
       <c r="F4" s="2">
@@ -2489,7 +2501,7 @@
       <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>2235489872</v>
       </c>
       <c r="F5" s="2">
@@ -2515,7 +2527,7 @@
       <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="3">
         <v>223155215730</v>
       </c>
       <c r="F6" s="2">
@@ -2541,7 +2553,7 @@
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>2234643873</v>
       </c>
       <c r="F7" s="2">
@@ -2567,7 +2579,7 @@
       <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>223156353455</v>
       </c>
       <c r="F8" s="2">
@@ -2593,7 +2605,7 @@
       <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>2235281771</v>
       </c>
       <c r="F9" s="2">
@@ -2619,7 +2631,7 @@
       <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>2358450436</v>
       </c>
       <c r="F10" s="2">
@@ -2645,7 +2657,7 @@
       <c r="D11" s="1" t="s">
         <v>522</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="3">
         <v>2356495090</v>
       </c>
       <c r="F11" s="2">
@@ -2671,7 +2683,7 @@
       <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>2473466738</v>
       </c>
       <c r="F12" s="2">
@@ -2697,7 +2709,7 @@
       <c r="D13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>2473505825</v>
       </c>
       <c r="F13" s="2">
@@ -2723,7 +2735,7 @@
       <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="3">
         <v>2358413870</v>
       </c>
       <c r="F14" s="2">
@@ -2749,7 +2761,7 @@
       <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <v>2364626006</v>
       </c>
       <c r="F15" s="2">
@@ -2775,7 +2787,7 @@
       <c r="D16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>2473468800</v>
       </c>
       <c r="F16" s="2">
@@ -2801,7 +2813,7 @@
       <c r="D17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="3">
         <v>2355530557</v>
       </c>
       <c r="F17" s="2">
@@ -2827,7 +2839,7 @@
       <c r="D18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="3">
         <v>2364342513</v>
       </c>
       <c r="F18" s="2">
@@ -2853,7 +2865,7 @@
       <c r="D19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="3">
         <v>2364534907</v>
       </c>
       <c r="F19" s="2">
@@ -2879,7 +2891,7 @@
       <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>2364628498</v>
       </c>
       <c r="F20" s="2">
@@ -2905,7 +2917,7 @@
       <c r="D21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>236154558780</v>
       </c>
       <c r="F21" s="2">
@@ -2931,7 +2943,7 @@
       <c r="D22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="3">
         <v>2473453540</v>
       </c>
       <c r="F22" s="2">
@@ -2957,7 +2969,7 @@
       <c r="D23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="3">
         <v>2364325229</v>
       </c>
       <c r="F23" s="2">
@@ -2983,7 +2995,7 @@
       <c r="D24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="3">
         <v>2355481843</v>
       </c>
       <c r="F24" s="2">
@@ -3009,7 +3021,7 @@
       <c r="D25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="3">
         <v>2364369342</v>
       </c>
       <c r="F25" s="2">
@@ -3035,7 +3047,7 @@
       <c r="D26" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="3">
         <v>2473504497</v>
       </c>
       <c r="F26" s="2">
@@ -3061,7 +3073,7 @@
       <c r="D27" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="3">
         <v>2364672255</v>
       </c>
       <c r="F27" s="2">
@@ -3087,7 +3099,7 @@
       <c r="D28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="3">
         <v>2473504261</v>
       </c>
       <c r="F28" s="2">
@@ -3113,7 +3125,7 @@
       <c r="D29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="3">
         <v>2356420680</v>
       </c>
       <c r="F29" s="2">
@@ -3139,7 +3151,7 @@
       <c r="D30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="3">
         <v>2364691174</v>
       </c>
       <c r="F30" s="2">
@@ -3165,7 +3177,7 @@
       <c r="D31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="3">
         <v>2355570428</v>
       </c>
       <c r="F31" s="2">
@@ -3191,7 +3203,7 @@
       <c r="D32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="3">
         <v>2355454644</v>
       </c>
       <c r="F32" s="2">
@@ -3217,7 +3229,7 @@
       <c r="D33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="3">
         <v>50710100</v>
       </c>
       <c r="F33" s="2">
@@ -3243,7 +3255,7 @@
       <c r="D34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="3">
         <v>1565701475</v>
       </c>
       <c r="F34" s="2">
@@ -3269,7 +3281,7 @@
       <c r="D35" s="1" t="s">
         <v>526</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="3">
         <v>45713185</v>
       </c>
       <c r="F35" s="2">
@@ -3295,7 +3307,7 @@
       <c r="D36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="3">
         <v>46831569</v>
       </c>
       <c r="F36" s="2">
@@ -3321,7 +3333,7 @@
       <c r="D37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="3">
         <v>32883528</v>
       </c>
       <c r="F37" s="2">
@@ -3347,7 +3359,7 @@
       <c r="D38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="3">
         <v>1531742276</v>
       </c>
       <c r="F38" s="2">
@@ -3373,7 +3385,7 @@
       <c r="D39" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="3">
         <v>1540875629</v>
       </c>
       <c r="F39" s="2">
@@ -3399,7 +3411,7 @@
       <c r="D40" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="3">
         <v>43822379</v>
       </c>
       <c r="F40" s="2">
@@ -3425,7 +3437,7 @@
       <c r="D41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="3">
         <v>1528181342</v>
       </c>
       <c r="F41" s="2">
@@ -3451,7 +3463,7 @@
       <c r="D42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="3">
         <v>46860395</v>
       </c>
       <c r="F42" s="2">
@@ -3477,7 +3489,7 @@
       <c r="D43" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="3">
         <v>1532317761</v>
       </c>
       <c r="F43" s="2">
@@ -3503,7 +3515,7 @@
       <c r="D44" s="1" t="s">
         <v>528</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="3">
         <v>1538276287</v>
       </c>
       <c r="F44" s="2">
@@ -3529,7 +3541,7 @@
       <c r="D45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="3">
         <v>1551247514</v>
       </c>
       <c r="F45" s="2">
@@ -3555,7 +3567,7 @@
       <c r="D46" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="3">
         <v>1568897979</v>
       </c>
       <c r="F46" s="2">
@@ -3581,7 +3593,7 @@
       <c r="D47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="3">
         <v>1521772922</v>
       </c>
       <c r="F47" s="2">
@@ -3607,7 +3619,7 @@
       <c r="D48" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="3">
         <v>1557817379</v>
       </c>
       <c r="F48" s="2">
@@ -3633,7 +3645,7 @@
       <c r="D49" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="3">
         <v>39640114</v>
       </c>
       <c r="F49" s="2">
@@ -3659,7 +3671,7 @@
       <c r="D50" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="3">
         <v>1540918562</v>
       </c>
       <c r="F50" s="2">
@@ -3685,7 +3697,7 @@
       <c r="D51" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="3">
         <v>1568731001</v>
       </c>
       <c r="F51" s="2">
@@ -3711,7 +3723,7 @@
       <c r="D52" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="3">
         <v>1537728310</v>
       </c>
       <c r="F52" s="2">
@@ -3737,7 +3749,7 @@
       <c r="D53" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="3">
         <v>1562260803</v>
       </c>
       <c r="F53" s="2">
@@ -3763,7 +3775,7 @@
       <c r="D54" s="1" t="s">
         <v>535</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="3">
         <v>1532481266</v>
       </c>
       <c r="F54" s="2">
@@ -3789,7 +3801,7 @@
       <c r="D55" s="1" t="s">
         <v>537</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="3">
         <v>1567034653</v>
       </c>
       <c r="F55" s="2">
@@ -3815,7 +3827,7 @@
       <c r="D56" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="3">
         <v>1527416558</v>
       </c>
       <c r="F56" s="2">
@@ -3841,7 +3853,7 @@
       <c r="D57" s="1" t="s">
         <v>539</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="3">
         <v>46014049</v>
       </c>
       <c r="F57" s="2">
@@ -3867,7 +3879,7 @@
       <c r="D58" s="1" t="s">
         <v>540</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="3">
         <v>1565741888</v>
       </c>
       <c r="F58" s="2">
@@ -3893,7 +3905,7 @@
       <c r="D59" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="3">
         <v>45662275</v>
       </c>
       <c r="F59" s="2">
@@ -3919,7 +3931,7 @@
       <c r="D60" s="1" t="s">
         <v>541</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="3">
         <v>1541936005</v>
       </c>
       <c r="F60" s="2">
@@ -3945,7 +3957,7 @@
       <c r="D61" s="1" t="s">
         <v>543</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="3">
         <v>1515636853</v>
       </c>
       <c r="F61" s="2">
@@ -3971,7 +3983,7 @@
       <c r="D62" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="3">
         <v>1558883099</v>
       </c>
       <c r="F62" s="2">
@@ -3997,7 +4009,7 @@
       <c r="D63" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="3">
         <v>1559542484</v>
       </c>
       <c r="F63" s="2">
@@ -4023,7 +4035,7 @@
       <c r="D64" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="3">
         <v>1560198719</v>
       </c>
       <c r="F64" s="2">
@@ -4049,7 +4061,7 @@
       <c r="D65" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="3">
         <v>156556280</v>
       </c>
       <c r="F65" s="2">
@@ -4075,7 +4087,7 @@
       <c r="D66" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="3">
         <v>1567035407</v>
       </c>
       <c r="F66" s="2">
@@ -4101,7 +4113,7 @@
       <c r="D67" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="3">
         <v>1562628100</v>
       </c>
       <c r="F67" s="2">
@@ -4127,7 +4139,7 @@
       <c r="D68" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="3">
         <v>42421753</v>
       </c>
       <c r="F68" s="2">
@@ -4153,7 +4165,7 @@
       <c r="D69" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="3">
         <v>1524503485</v>
       </c>
       <c r="F69" s="2">
@@ -4179,7 +4191,7 @@
       <c r="D70" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="3">
         <v>49022146</v>
       </c>
       <c r="F70" s="2">
@@ -4205,7 +4217,7 @@
       <c r="D71" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="3">
         <v>1554717335</v>
       </c>
       <c r="F71" s="2">
@@ -4231,7 +4243,7 @@
       <c r="D72" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="3">
         <v>1558269777</v>
       </c>
       <c r="F72" s="2">
@@ -4257,7 +4269,7 @@
       <c r="D73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="3">
         <v>1551310126</v>
       </c>
       <c r="F73" s="2">
@@ -4283,7 +4295,7 @@
       <c r="D74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="3">
         <v>1555673099</v>
       </c>
       <c r="F74" s="2">
@@ -4309,7 +4321,7 @@
       <c r="D75" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="3">
         <v>1562877398</v>
       </c>
       <c r="F75" s="2">
@@ -4335,7 +4347,7 @@
       <c r="D76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="3">
         <v>1564958459</v>
       </c>
       <c r="F76" s="2">
@@ -4361,7 +4373,7 @@
       <c r="D77" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="3">
         <v>15143134758</v>
       </c>
       <c r="F77" s="2">
@@ -4387,7 +4399,7 @@
       <c r="D78" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="3">
         <v>1539697832</v>
       </c>
       <c r="F78" s="2">
@@ -4413,7 +4425,7 @@
       <c r="D79" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="3">
         <v>1544281075</v>
       </c>
       <c r="F79" s="2">
@@ -4439,7 +4451,7 @@
       <c r="D80" s="1" t="s">
         <v>554</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="3">
         <v>1542888893</v>
       </c>
       <c r="F80" s="2">
@@ -4465,7 +4477,7 @@
       <c r="D81" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E81" s="3">
         <v>1149357036</v>
       </c>
       <c r="F81" s="2">
@@ -4491,7 +4503,7 @@
       <c r="D82" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E82" s="3">
         <v>1531510769</v>
       </c>
       <c r="F82" s="2">
@@ -4517,7 +4529,7 @@
       <c r="D83" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="3">
         <v>1536506226</v>
       </c>
       <c r="F83" s="2">
@@ -4543,7 +4555,7 @@
       <c r="D84" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E84" s="1">
+      <c r="E84" s="3">
         <v>1553690018</v>
       </c>
       <c r="F84" s="2">
@@ -4569,7 +4581,7 @@
       <c r="D85" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E85" s="3">
         <v>1569601704</v>
       </c>
       <c r="F85" s="2">
@@ -4595,7 +4607,7 @@
       <c r="D86" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E86" s="3">
         <v>1564020726</v>
       </c>
       <c r="F86" s="2">
@@ -4621,7 +4633,7 @@
       <c r="D87" s="1" t="s">
         <v>555</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E87" s="3">
         <v>1536542817</v>
       </c>
       <c r="F87" s="2">
@@ -4647,7 +4659,7 @@
       <c r="D88" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E88" s="3">
         <v>42671549</v>
       </c>
       <c r="F88" s="2">
@@ -4673,7 +4685,7 @@
       <c r="D89" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E89" s="3">
         <v>1542641097</v>
       </c>
       <c r="F89" s="2">
@@ -4699,7 +4711,7 @@
       <c r="D90" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E90" s="3">
         <v>1533822246</v>
       </c>
       <c r="F90" s="2">
@@ -4725,7 +4737,7 @@
       <c r="D91" s="1" t="s">
         <v>556</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E91" s="3">
         <v>1540610713</v>
       </c>
       <c r="F91" s="2">
@@ -4751,7 +4763,7 @@
       <c r="D92" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E92" s="1">
+      <c r="E92" s="3">
         <v>1505440295</v>
       </c>
       <c r="F92" s="2">
@@ -4777,7 +4789,7 @@
       <c r="D93" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="E93" s="1">
+      <c r="E93" s="3">
         <v>1539266463</v>
       </c>
       <c r="F93" s="2">
@@ -4803,7 +4815,7 @@
       <c r="D94" s="1" t="s">
         <v>557</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E94" s="3">
         <v>1530650932</v>
       </c>
       <c r="F94" s="2">
@@ -4829,7 +4841,7 @@
       <c r="D95" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E95" s="3">
         <v>1542307184</v>
       </c>
       <c r="F95" s="2">
@@ -4855,7 +4867,7 @@
       <c r="D96" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E96" s="3">
         <v>1552221714</v>
       </c>
       <c r="F96" s="2">
@@ -4881,7 +4893,7 @@
       <c r="D97" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="E97" s="1">
+      <c r="E97" s="3">
         <v>1559375723</v>
       </c>
       <c r="F97" s="2">
@@ -4907,7 +4919,7 @@
       <c r="D98" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E98" s="3">
         <v>1565663772</v>
       </c>
       <c r="F98" s="2">
@@ -4933,7 +4945,7 @@
       <c r="D99" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E99" s="1">
+      <c r="E99" s="3">
         <v>1166624135</v>
       </c>
       <c r="F99" s="2">
@@ -4959,7 +4971,7 @@
       <c r="D100" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E100" s="3">
         <v>1527582705</v>
       </c>
       <c r="F100" s="2">
@@ -4985,7 +4997,7 @@
       <c r="D101" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E101" s="1">
+      <c r="E101" s="3">
         <v>1530034132</v>
       </c>
       <c r="F101" s="2">
@@ -5011,7 +5023,7 @@
       <c r="D102" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E102" s="1">
+      <c r="E102" s="3">
         <v>1522763938</v>
       </c>
       <c r="F102" s="2">
@@ -5037,7 +5049,7 @@
       <c r="D103" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E103" s="1">
+      <c r="E103" s="3">
         <v>1567624176</v>
       </c>
       <c r="F103" s="2">
@@ -5063,7 +5075,7 @@
       <c r="D104" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E104" s="1">
+      <c r="E104" s="3">
         <v>1562371704</v>
       </c>
       <c r="F104" s="2">
@@ -5089,7 +5101,7 @@
       <c r="D105" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E105" s="1">
+      <c r="E105" s="3">
         <v>1553264029</v>
       </c>
       <c r="F105" s="2">
@@ -5115,7 +5127,7 @@
       <c r="D106" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E106" s="1">
+      <c r="E106" s="3">
         <v>1554882858</v>
       </c>
       <c r="F106" s="2">
@@ -5141,7 +5153,7 @@
       <c r="D107" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="E107" s="1">
+      <c r="E107" s="3">
         <v>42318499</v>
       </c>
       <c r="F107" s="2">
@@ -5167,7 +5179,7 @@
       <c r="D108" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E108" s="1">
+      <c r="E108" s="3">
         <v>42304571</v>
       </c>
       <c r="F108" s="2">
@@ -5193,7 +5205,7 @@
       <c r="D109" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E109" s="1">
+      <c r="E109" s="3">
         <v>1520658960</v>
       </c>
       <c r="F109" s="2">
@@ -5219,7 +5231,7 @@
       <c r="D110" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E110" s="1">
+      <c r="E110" s="3">
         <v>1560382907</v>
       </c>
       <c r="F110" s="2">
@@ -5245,7 +5257,7 @@
       <c r="D111" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="E111" s="1">
+      <c r="E111" s="3">
         <v>42418533</v>
       </c>
       <c r="F111" s="2">
@@ -5271,7 +5283,7 @@
       <c r="D112" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E112" s="1">
+      <c r="E112" s="3">
         <v>1532143002</v>
       </c>
       <c r="F112" s="2">
@@ -5297,7 +5309,7 @@
       <c r="D113" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E113" s="1">
+      <c r="E113" s="3">
         <v>1534643915</v>
       </c>
       <c r="F113" s="2">
@@ -5323,7 +5335,7 @@
       <c r="D114" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E114" s="1">
+      <c r="E114" s="3">
         <v>1527947401</v>
       </c>
       <c r="F114" s="2">
@@ -5349,7 +5361,7 @@
       <c r="D115" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E115" s="1">
+      <c r="E115" s="3">
         <v>1568573277</v>
       </c>
       <c r="F115" s="2">
@@ -5375,7 +5387,7 @@
       <c r="D116" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E116" s="1">
+      <c r="E116" s="3">
         <v>1524803427</v>
       </c>
       <c r="F116" s="2">
@@ -5401,7 +5413,7 @@
       <c r="D117" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E117" s="3">
         <v>1542083170</v>
       </c>
       <c r="F117" s="2">
@@ -5427,7 +5439,7 @@
       <c r="D118" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E118" s="1">
+      <c r="E118" s="3">
         <v>1532103401</v>
       </c>
       <c r="F118" s="2">
@@ -5453,7 +5465,7 @@
       <c r="D119" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E119" s="1">
+      <c r="E119" s="3">
         <v>1564068610</v>
       </c>
       <c r="F119" s="2">
@@ -5479,7 +5491,7 @@
       <c r="D120" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E120" s="1">
+      <c r="E120" s="3">
         <v>42093716</v>
       </c>
       <c r="F120" s="2">
@@ -5505,7 +5517,7 @@
       <c r="D121" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E121" s="3">
         <v>1553478392</v>
       </c>
       <c r="F121" s="2">
@@ -5531,7 +5543,7 @@
       <c r="D122" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E122" s="1">
+      <c r="E122" s="3">
         <v>1559133126</v>
       </c>
       <c r="F122" s="2">
@@ -5557,7 +5569,7 @@
       <c r="D123" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="3">
         <v>1537822860</v>
       </c>
       <c r="F123" s="2">
@@ -5583,7 +5595,7 @@
       <c r="D124" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="E124" s="1">
+      <c r="E124" s="3">
         <v>1556436364</v>
       </c>
       <c r="F124" s="2">
@@ -5609,7 +5621,7 @@
       <c r="D125" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E125" s="1">
+      <c r="E125" s="3">
         <v>1542936740</v>
       </c>
       <c r="F125" s="2">
@@ -5635,7 +5647,7 @@
       <c r="D126" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126" s="3">
         <v>42092864</v>
       </c>
       <c r="F126" s="2">
@@ -5661,7 +5673,7 @@
       <c r="D127" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E127" s="1">
+      <c r="E127" s="3">
         <v>1543534167</v>
       </c>
       <c r="F127" s="2">
@@ -5687,7 +5699,7 @@
       <c r="D128" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E128" s="1">
+      <c r="E128" s="3">
         <v>1557522541</v>
       </c>
       <c r="F128" s="2">
@@ -5713,7 +5725,7 @@
       <c r="D129" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E129" s="1">
+      <c r="E129" s="3">
         <v>1542647000</v>
       </c>
       <c r="F129" s="2">
@@ -5739,7 +5751,7 @@
       <c r="D130" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="E130" s="1">
+      <c r="E130" s="3">
         <v>1542687166</v>
       </c>
       <c r="F130" s="2">
@@ -5765,7 +5777,7 @@
       <c r="D131" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E131" s="1">
+      <c r="E131" s="3">
         <v>42671549</v>
       </c>
       <c r="F131" s="2">
@@ -5791,7 +5803,7 @@
       <c r="D132" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E132" s="1">
+      <c r="E132" s="3">
         <v>1535992828</v>
       </c>
       <c r="F132" s="2">
@@ -5817,7 +5829,7 @@
       <c r="D133" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E133" s="1">
+      <c r="E133" s="3">
         <v>1541802875</v>
       </c>
       <c r="F133" s="2">
@@ -5843,7 +5855,7 @@
       <c r="D134" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E134" s="1">
+      <c r="E134" s="3">
         <v>1522023657</v>
       </c>
       <c r="F134" s="2">
@@ -5869,7 +5881,7 @@
       <c r="D135" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E135" s="1">
+      <c r="E135" s="3">
         <v>1520761157</v>
       </c>
       <c r="F135" s="2">
@@ -5895,7 +5907,7 @@
       <c r="D136" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E136" s="1">
+      <c r="E136" s="3">
         <v>42447385</v>
       </c>
       <c r="F136" s="2">
@@ -5921,7 +5933,7 @@
       <c r="D137" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E137" s="1">
+      <c r="E137" s="3">
         <v>1542856548</v>
       </c>
       <c r="F137" s="2">
@@ -5947,7 +5959,7 @@
       <c r="D138" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E138" s="1">
+      <c r="E138" s="3">
         <v>1554906729</v>
       </c>
       <c r="F138" s="2">
@@ -5973,7 +5985,7 @@
       <c r="D139" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E139" s="1">
+      <c r="E139" s="3">
         <v>42223568</v>
       </c>
       <c r="F139" s="2">
@@ -5999,7 +6011,7 @@
       <c r="D140" s="1" t="s">
         <v>569</v>
       </c>
-      <c r="E140" s="1">
+      <c r="E140" s="3">
         <v>1533123145</v>
       </c>
       <c r="F140" s="2">
@@ -6025,7 +6037,7 @@
       <c r="D141" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E141" s="1">
+      <c r="E141" s="3">
         <v>1542084861</v>
       </c>
       <c r="F141" s="2">
@@ -6051,7 +6063,7 @@
       <c r="D142" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="E142" s="1">
+      <c r="E142" s="3">
         <v>1527285654</v>
       </c>
       <c r="F142" s="2">
@@ -6077,7 +6089,7 @@
       <c r="D143" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E143" s="1">
+      <c r="E143" s="3">
         <v>42980478</v>
       </c>
       <c r="F143" s="2">
@@ -6103,7 +6115,7 @@
       <c r="D144" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E144" s="1" t="s">
+      <c r="E144" s="3" t="s">
         <v>253</v>
       </c>
       <c r="F144" s="2">
@@ -6129,7 +6141,7 @@
       <c r="D145" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E145" s="1">
+      <c r="E145" s="3">
         <v>1542810189</v>
       </c>
       <c r="F145" s="2">
@@ -6155,7 +6167,7 @@
       <c r="D146" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E146" s="1">
+      <c r="E146" s="3">
         <v>1566435333</v>
       </c>
       <c r="F146" s="2">
@@ -6181,7 +6193,7 @@
       <c r="D147" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E147" s="1">
+      <c r="E147" s="3">
         <v>15420017474</v>
       </c>
       <c r="F147" s="2">
@@ -6207,7 +6219,7 @@
       <c r="D148" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="E148" s="1">
+      <c r="E148" s="3">
         <v>1542896606</v>
       </c>
       <c r="F148" s="2">
@@ -6233,7 +6245,7 @@
       <c r="D149" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E149" s="1">
+      <c r="E149" s="3">
         <v>1542316155</v>
       </c>
       <c r="F149" s="2">
@@ -6259,7 +6271,7 @@
       <c r="D150" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="E150" s="1">
+      <c r="E150" s="3">
         <v>42434940</v>
       </c>
       <c r="F150" s="2">
@@ -6285,7 +6297,7 @@
       <c r="D151" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E151" s="1">
+      <c r="E151" s="3">
         <v>42180306</v>
       </c>
       <c r="F151" s="2">
@@ -6311,7 +6323,7 @@
       <c r="D152" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E152" s="1">
+      <c r="E152" s="3">
         <v>1146932393</v>
       </c>
       <c r="F152" s="2">
@@ -6337,7 +6349,7 @@
       <c r="D153" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E153" s="1">
+      <c r="E153" s="3">
         <v>15533580812</v>
       </c>
       <c r="F153" s="2">
@@ -6363,7 +6375,7 @@
       <c r="D154" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="E154" s="1">
+      <c r="E154" s="3">
         <v>1540542645</v>
       </c>
       <c r="F154" s="2">
@@ -6389,7 +6401,7 @@
       <c r="D155" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E155" s="1" t="s">
+      <c r="E155" s="3" t="s">
         <v>274</v>
       </c>
       <c r="F155" s="2">
@@ -6415,7 +6427,7 @@
       <c r="D156" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E156" s="1">
+      <c r="E156" s="3">
         <v>1554556401</v>
       </c>
       <c r="F156" s="2">
@@ -6441,7 +6453,7 @@
       <c r="D157" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E157" s="1">
+      <c r="E157" s="3">
         <v>1557968881</v>
       </c>
       <c r="F157" s="2">
@@ -6467,7 +6479,7 @@
       <c r="D158" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="E158" s="1">
+      <c r="E158" s="3">
         <v>1531714683</v>
       </c>
       <c r="F158" s="2">
@@ -6493,7 +6505,7 @@
       <c r="D159" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E159" s="1">
+      <c r="E159" s="3">
         <v>1559227505</v>
       </c>
       <c r="F159" s="2">
@@ -6519,7 +6531,7 @@
       <c r="D160" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E160" s="1">
+      <c r="E160" s="3">
         <v>1555673099</v>
       </c>
       <c r="F160" s="2">
@@ -6545,7 +6557,7 @@
       <c r="D161" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E161" s="1">
+      <c r="E161" s="3">
         <v>1561886761</v>
       </c>
       <c r="F161" s="2">
@@ -6571,7 +6583,7 @@
       <c r="D162" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E162" s="1">
+      <c r="E162" s="3">
         <v>1554137337</v>
       </c>
       <c r="F162" s="2">
@@ -6597,7 +6609,7 @@
       <c r="D163" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E163" s="1">
+      <c r="E163" s="3">
         <v>1554540390</v>
       </c>
       <c r="F163" s="2">
@@ -6623,7 +6635,7 @@
       <c r="D164" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E164" s="1">
+      <c r="E164" s="3">
         <v>1562671819</v>
       </c>
       <c r="F164" s="2">
@@ -6649,7 +6661,7 @@
       <c r="D165" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E165" s="1">
+      <c r="E165" s="3">
         <v>1549720330</v>
       </c>
       <c r="F165" s="2">
@@ -6675,7 +6687,7 @@
       <c r="D166" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="E166" s="1">
+      <c r="E166" s="3">
         <v>1555634555</v>
       </c>
       <c r="F166" s="2">
@@ -6701,7 +6713,7 @@
       <c r="D167" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E167" s="1" t="s">
+      <c r="E167" s="3" t="s">
         <v>299</v>
       </c>
       <c r="F167" s="2">
@@ -6727,7 +6739,7 @@
       <c r="D168" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E168" s="1">
+      <c r="E168" s="3">
         <v>1569738443</v>
       </c>
       <c r="F168" s="2">
@@ -6753,7 +6765,7 @@
       <c r="D169" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E169" s="1" t="s">
+      <c r="E169" s="3" t="s">
         <v>304</v>
       </c>
       <c r="F169" s="2">
@@ -6779,7 +6791,7 @@
       <c r="D170" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E170" s="1">
+      <c r="E170" s="3">
         <v>1533572664</v>
       </c>
       <c r="F170" s="2">
@@ -6805,7 +6817,7 @@
       <c r="D171" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E171" s="1" t="s">
+      <c r="E171" s="3" t="s">
         <v>309</v>
       </c>
       <c r="F171" s="2">
@@ -6831,7 +6843,7 @@
       <c r="D172" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="E172" s="1">
+      <c r="E172" s="3">
         <v>1546425831</v>
       </c>
       <c r="F172" s="2">
@@ -6857,7 +6869,7 @@
       <c r="D173" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="E173" s="1">
+      <c r="E173" s="3">
         <v>1561814891</v>
       </c>
       <c r="F173" s="2">
@@ -6883,7 +6895,7 @@
       <c r="D174" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="E174" s="1">
+      <c r="E174" s="3">
         <v>1554204385</v>
       </c>
       <c r="F174" s="2">
@@ -6909,7 +6921,7 @@
       <c r="D175" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E175" s="1">
+      <c r="E175" s="3">
         <v>1533865556</v>
       </c>
       <c r="F175" s="2">
@@ -6935,7 +6947,7 @@
       <c r="D176" s="1" t="s">
         <v>572</v>
       </c>
-      <c r="E176" s="1" t="s">
+      <c r="E176" s="3" t="s">
         <v>319</v>
       </c>
       <c r="F176" s="2">
@@ -6961,7 +6973,7 @@
       <c r="D177" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E177" s="1">
+      <c r="E177" s="3">
         <v>1522964106</v>
       </c>
       <c r="F177" s="2">
@@ -6987,7 +6999,7 @@
       <c r="D178" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="E178" s="1" t="s">
+      <c r="E178" s="3" t="s">
         <v>324</v>
       </c>
       <c r="F178" s="2">
@@ -7013,7 +7025,7 @@
       <c r="D179" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="E179" s="1">
+      <c r="E179" s="3">
         <v>1544943344</v>
       </c>
       <c r="F179" s="2">
@@ -7039,7 +7051,7 @@
       <c r="D180" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="E180" s="1">
+      <c r="E180" s="3">
         <v>1563245921</v>
       </c>
       <c r="F180" s="2">
@@ -7065,7 +7077,7 @@
       <c r="D181" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="E181" s="1">
+      <c r="E181" s="3">
         <v>1556645118</v>
       </c>
       <c r="F181" s="2">
@@ -7091,7 +7103,7 @@
       <c r="D182" s="1" t="s">
         <v>573</v>
       </c>
-      <c r="E182" s="1">
+      <c r="E182" s="3">
         <v>1550221532</v>
       </c>
       <c r="F182" s="2">
@@ -7117,7 +7129,7 @@
       <c r="D183" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="E183" s="1">
+      <c r="E183" s="3">
         <v>1539781980</v>
       </c>
       <c r="F183" s="2">
@@ -7143,7 +7155,7 @@
       <c r="D184" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E184" s="1">
+      <c r="E184" s="3">
         <v>1537817155</v>
       </c>
       <c r="F184" s="2">
@@ -7169,7 +7181,7 @@
       <c r="D185" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="E185" s="1">
+      <c r="E185" s="3">
         <v>123456</v>
       </c>
       <c r="F185" s="2">
@@ -7195,7 +7207,7 @@
       <c r="D186" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E186" s="1">
+      <c r="E186" s="3">
         <v>1136506226</v>
       </c>
       <c r="F186" s="2">
@@ -7221,7 +7233,7 @@
       <c r="D187" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E187" s="1">
+      <c r="E187" s="3">
         <v>1142307184</v>
       </c>
       <c r="F187" s="2">
@@ -7247,7 +7259,7 @@
       <c r="D188" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E188" s="1">
+      <c r="E188" s="3">
         <v>1164020726</v>
       </c>
       <c r="F188" s="2">
@@ -7273,7 +7285,7 @@
       <c r="D189" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E189" s="1">
+      <c r="E189" s="3">
         <v>1166624135</v>
       </c>
       <c r="F189" s="2">
@@ -7299,7 +7311,7 @@
       <c r="D190" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="E190" s="1">
+      <c r="E190" s="3">
         <v>1569738443</v>
       </c>
       <c r="F190" s="2">
@@ -7325,7 +7337,7 @@
       <c r="D191" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="E191" s="1">
+      <c r="E191" s="3">
         <v>42418533</v>
       </c>
       <c r="F191" s="2">
@@ -7351,7 +7363,7 @@
       <c r="D192" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E192" s="1">
+      <c r="E192" s="3">
         <v>42304571</v>
       </c>
       <c r="F192" s="2">
@@ -7377,7 +7389,7 @@
       <c r="D193" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E193" s="1">
+      <c r="E193" s="3">
         <v>1153478392</v>
       </c>
       <c r="F193" s="2">
@@ -7403,7 +7415,7 @@
       <c r="D194" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E194" s="1">
+      <c r="E194" s="3">
         <v>1169535957</v>
       </c>
       <c r="F194" s="2">
@@ -7429,7 +7441,7 @@
       <c r="D195" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="E195" s="1">
+      <c r="E195" s="3">
         <v>1127285654</v>
       </c>
       <c r="F195" s="2">
@@ -7455,7 +7467,7 @@
       <c r="D196" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="E196" s="1">
+      <c r="E196" s="3">
         <v>1136387283</v>
       </c>
       <c r="F196" s="2">
@@ -7481,7 +7493,7 @@
       <c r="D197" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E197" s="1">
+      <c r="E197" s="3">
         <v>11420017474</v>
       </c>
       <c r="F197" s="2">
@@ -7507,7 +7519,7 @@
       <c r="D198" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E198" s="1">
+      <c r="E198" s="3">
         <v>1153134144</v>
       </c>
       <c r="F198" s="2">
@@ -7533,7 +7545,7 @@
       <c r="D199" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E199" s="1">
+      <c r="E199" s="3">
         <v>1131742276</v>
       </c>
       <c r="F199" s="2">
@@ -7559,7 +7571,7 @@
       <c r="D200" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="E200" s="1">
+      <c r="E200" s="3">
         <v>43822379</v>
       </c>
       <c r="F200" s="2">
@@ -7585,7 +7597,7 @@
       <c r="D201" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="E201" s="1">
+      <c r="E201" s="3">
         <v>1559227505</v>
       </c>
       <c r="F201" s="2">
@@ -7611,7 +7623,7 @@
       <c r="D202" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="E202" s="1">
+      <c r="E202" s="3">
         <v>45829355</v>
       </c>
       <c r="F202" s="2">
@@ -7637,7 +7649,7 @@
       <c r="D203" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="E203" s="1">
+      <c r="E203" s="3">
         <v>1162282632</v>
       </c>
       <c r="F203" s="2">
@@ -7663,7 +7675,7 @@
       <c r="D204" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="E204" s="1">
+      <c r="E204" s="3">
         <v>45019297</v>
       </c>
       <c r="F204" s="2">
@@ -7689,7 +7701,7 @@
       <c r="D205" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="E205" s="1">
+      <c r="E205" s="3">
         <v>1144943344</v>
       </c>
       <c r="F205" s="2">
@@ -7715,7 +7727,7 @@
       <c r="D206" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="E206" s="1">
+      <c r="E206" s="3">
         <v>1168897979</v>
       </c>
       <c r="F206" s="2">
@@ -7741,7 +7753,7 @@
       <c r="D207" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="E207" s="1">
+      <c r="E207" s="3">
         <v>46861584</v>
       </c>
       <c r="F207" s="2">
@@ -7767,7 +7779,7 @@
       <c r="D208" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E208" s="1">
+      <c r="E208" s="3">
         <v>1140918562</v>
       </c>
       <c r="F208" s="2">
@@ -7793,7 +7805,7 @@
       <c r="D209" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E209" s="1">
+      <c r="E209" s="3">
         <v>1164958459</v>
       </c>
       <c r="F209" s="2">
@@ -7819,7 +7831,7 @@
       <c r="D210" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="E210" s="1">
+      <c r="E210" s="3">
         <v>1121714716</v>
       </c>
       <c r="F210" s="2">
@@ -7845,7 +7857,7 @@
       <c r="D211" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="E211" s="1">
+      <c r="E211" s="3">
         <v>48964807</v>
       </c>
       <c r="F211" s="2">
@@ -7871,7 +7883,7 @@
       <c r="D212" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E212" s="1">
+      <c r="E212" s="3">
         <v>2358413870</v>
       </c>
       <c r="F212" s="2">
@@ -7897,7 +7909,7 @@
       <c r="D213" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="E213" s="1">
+      <c r="E213" s="3">
         <v>2473468800</v>
       </c>
       <c r="F213" s="2">
@@ -7923,7 +7935,7 @@
       <c r="D214" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E214" s="1">
+      <c r="E214" s="3">
         <v>2364342513</v>
       </c>
       <c r="F214" s="2">
@@ -7949,7 +7961,7 @@
       <c r="D215" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E215" s="1">
+      <c r="E215" s="3">
         <v>2364628498</v>
       </c>
       <c r="F215" s="2">
@@ -7975,7 +7987,7 @@
       <c r="D216" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="E216" s="1">
+      <c r="E216" s="3">
         <v>2355454644</v>
       </c>
       <c r="F216" s="2">
@@ -8001,7 +8013,7 @@
       <c r="D217" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="E217" s="1">
+      <c r="E217" s="3">
         <v>1532262983</v>
       </c>
       <c r="F217" s="2">
@@ -8027,7 +8039,7 @@
       <c r="D218" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="E218" s="1">
+      <c r="E218" s="3">
         <v>1157406463</v>
       </c>
       <c r="F218" s="2">
@@ -8053,7 +8065,7 @@
       <c r="D219" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E219" s="1">
+      <c r="E219" s="3">
         <v>1121926069</v>
       </c>
       <c r="F219" s="2">
@@ -8079,7 +8091,7 @@
       <c r="D220" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="E220" s="1">
+      <c r="E220" s="3">
         <v>1130106568</v>
       </c>
       <c r="F220" s="2">
@@ -8105,7 +8117,7 @@
       <c r="D221" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="E221" s="1">
+      <c r="E221" s="3">
         <v>1122354593</v>
       </c>
       <c r="F221" s="2">
@@ -8131,7 +8143,7 @@
       <c r="D222" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="E222" s="1">
+      <c r="E222" s="3">
         <v>1132088855</v>
       </c>
       <c r="F222" s="2">
@@ -8157,7 +8169,7 @@
       <c r="D223" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="E223" s="1">
+      <c r="E223" s="3">
         <v>1161591080</v>
       </c>
       <c r="F223" s="2">
@@ -8183,7 +8195,7 @@
       <c r="D224" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E224" s="1">
+      <c r="E224" s="3">
         <v>20578201</v>
       </c>
       <c r="F224" s="2">
@@ -8209,7 +8221,7 @@
       <c r="D225" s="1" t="s">
         <v>575</v>
       </c>
-      <c r="E225" s="1">
+      <c r="E225" s="3">
         <v>1175329776</v>
       </c>
       <c r="F225" s="2">
@@ -8235,7 +8247,7 @@
       <c r="D226" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E226" s="1">
+      <c r="E226" s="3">
         <v>1139410663</v>
       </c>
       <c r="F226" s="2">
@@ -8261,7 +8273,7 @@
       <c r="D227" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="E227" s="1">
+      <c r="E227" s="3">
         <v>2234911781</v>
       </c>
       <c r="F227" s="2">
@@ -8287,7 +8299,7 @@
       <c r="D228" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E228" s="1">
+      <c r="E228" s="3">
         <v>2235692017</v>
       </c>
       <c r="F228" s="2">
@@ -8313,7 +8325,7 @@
       <c r="D229" s="1" t="s">
         <v>392</v>
       </c>
-      <c r="E229" s="1">
+      <c r="E229" s="3">
         <v>2234944988</v>
       </c>
       <c r="F229" s="2">
@@ -8339,7 +8351,7 @@
       <c r="D230" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E230" s="1">
+      <c r="E230" s="3">
         <v>2364691174</v>
       </c>
       <c r="F230" s="2">
@@ -8365,7 +8377,7 @@
       <c r="D231" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="E231" s="1">
+      <c r="E231" s="3">
         <v>2473506654</v>
       </c>
       <c r="F231" s="2">
@@ -8391,7 +8403,7 @@
       <c r="D232" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="E232" s="1">
+      <c r="E232" s="3">
         <v>2364536647</v>
       </c>
       <c r="F232" s="2">
@@ -8417,7 +8429,7 @@
       <c r="D233" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="E233" s="1">
+      <c r="E233" s="3">
         <v>2364695067</v>
       </c>
       <c r="F233" s="2">
@@ -8443,7 +8455,7 @@
       <c r="D234" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="E234" s="1">
+      <c r="E234" s="3">
         <v>2473414836</v>
       </c>
       <c r="F234" s="2">
@@ -8469,7 +8481,7 @@
       <c r="D235" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="E235" s="1">
+      <c r="E235" s="3">
         <v>2355647467</v>
       </c>
       <c r="F235" s="2">
@@ -8495,7 +8507,7 @@
       <c r="D236" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="E236" s="1">
+      <c r="E236" s="3">
         <v>236114653725</v>
       </c>
       <c r="F236" s="2">
@@ -8521,7 +8533,7 @@
       <c r="D237" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="E237" s="1">
+      <c r="E237" s="3">
         <v>1131727529</v>
       </c>
       <c r="F237" s="2">
@@ -8547,7 +8559,7 @@
       <c r="D238" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="E238" s="1">
+      <c r="E238" s="3">
         <v>1168349347</v>
       </c>
       <c r="F238" s="2">
@@ -8573,7 +8585,7 @@
       <c r="D239" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="E239" s="1">
+      <c r="E239" s="3">
         <v>1144499125</v>
       </c>
       <c r="F239" s="2">
@@ -8599,7 +8611,7 @@
       <c r="D240" s="1" t="s">
         <v>412</v>
       </c>
-      <c r="E240" s="1">
+      <c r="E240" s="3">
         <v>1158094830</v>
       </c>
       <c r="F240" s="2">
@@ -8625,7 +8637,7 @@
       <c r="D241" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="E241" s="1">
+      <c r="E241" s="3">
         <v>1130840425</v>
       </c>
       <c r="F241" s="2">
@@ -8651,7 +8663,7 @@
       <c r="D242" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="E242" s="1">
+      <c r="E242" s="3">
         <v>47864782</v>
       </c>
       <c r="F242" s="2">
@@ -8677,7 +8689,7 @@
       <c r="D243" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="E243" s="1">
+      <c r="E243" s="3">
         <v>49418323</v>
       </c>
       <c r="F243" s="2">
@@ -8703,7 +8715,7 @@
       <c r="D244" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="E244" s="1">
+      <c r="E244" s="3">
         <v>1126532823</v>
       </c>
       <c r="F244" s="2">
@@ -8729,7 +8741,7 @@
       <c r="D245" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="E245" s="1">
+      <c r="E245" s="3">
         <v>40507441</v>
       </c>
       <c r="F245" s="2">
@@ -8755,7 +8767,7 @@
       <c r="D246" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="E246" s="1">
+      <c r="E246" s="3">
         <v>46425799</v>
       </c>
       <c r="F246" s="2">
@@ -8781,7 +8793,7 @@
       <c r="D247" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="E247" s="1">
+      <c r="E247" s="3">
         <v>1157014091</v>
       </c>
       <c r="F247" s="2">
@@ -8807,7 +8819,7 @@
       <c r="D248" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="E248" s="1">
+      <c r="E248" s="3">
         <v>1160209684</v>
       </c>
       <c r="F248" s="2">
@@ -8833,7 +8845,7 @@
       <c r="D249" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="E249" s="1">
+      <c r="E249" s="3">
         <v>1547746849</v>
       </c>
       <c r="F249" s="2">
@@ -8859,7 +8871,7 @@
       <c r="D250" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="E250" s="1">
+      <c r="E250" s="3">
         <v>49415750</v>
       </c>
       <c r="F250" s="2">
@@ -8885,7 +8897,7 @@
       <c r="D251" s="1" t="s">
         <v>433</v>
       </c>
-      <c r="E251" s="1">
+      <c r="E251" s="3">
         <v>1154294603</v>
       </c>
       <c r="F251" s="2">
@@ -8911,7 +8923,7 @@
       <c r="D252" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="E252" s="1">
+      <c r="E252" s="3">
         <v>1160642617</v>
       </c>
       <c r="F252" s="2">
@@ -8937,7 +8949,7 @@
       <c r="D253" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="E253" s="1">
+      <c r="E253" s="3">
         <v>1155833913</v>
       </c>
       <c r="F253" s="2">
@@ -8963,7 +8975,7 @@
       <c r="D254" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="E254" s="1">
+      <c r="E254" s="3">
         <v>1148548663</v>
       </c>
       <c r="F254" s="2">
@@ -8989,7 +9001,7 @@
       <c r="D255" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="E255" s="1">
+      <c r="E255" s="3">
         <v>1169585595</v>
       </c>
       <c r="F255" s="2">
@@ -9015,7 +9027,7 @@
       <c r="D256" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="E256" s="1">
+      <c r="E256" s="3">
         <v>2473406671</v>
       </c>
       <c r="F256" s="2">
@@ -9041,7 +9053,7 @@
       <c r="D257" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="E257" s="1">
+      <c r="E257" s="3">
         <v>2355677760</v>
       </c>
       <c r="F257" s="2">
@@ -9067,7 +9079,7 @@
       <c r="D258" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="E258" s="1">
+      <c r="E258" s="3">
         <v>2364414744</v>
       </c>
       <c r="F258" s="2">
@@ -9093,7 +9105,7 @@
       <c r="D259" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="E259" s="1">
+      <c r="E259" s="3">
         <v>22315514706</v>
       </c>
       <c r="F259" s="2">
@@ -9119,7 +9131,7 @@
       <c r="D260" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="E260" s="1">
+      <c r="E260" s="3">
         <v>1142282776</v>
       </c>
       <c r="F260" s="2">
@@ -9145,7 +9157,7 @@
       <c r="D261" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="E261" s="1">
+      <c r="E261" s="3">
         <v>1159958884</v>
       </c>
       <c r="F261" s="2">
@@ -9171,7 +9183,7 @@
       <c r="D262" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="E262" s="1">
+      <c r="E262" s="3">
         <v>1165119970</v>
       </c>
       <c r="F262" s="1" t="s">
@@ -9197,7 +9209,7 @@
       <c r="D263" s="1" t="s">
         <v>577</v>
       </c>
-      <c r="E263" s="1">
+      <c r="E263" s="3">
         <v>25721977</v>
       </c>
       <c r="F263" s="2">
@@ -9223,7 +9235,7 @@
       <c r="D264" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E264" s="1">
+      <c r="E264" s="3">
         <v>1135056311</v>
       </c>
       <c r="F264" s="2">
@@ -9249,7 +9261,7 @@
       <c r="D265" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="E265" s="1">
+      <c r="E265" s="3">
         <v>1567031389</v>
       </c>
       <c r="F265" s="2">
@@ -9275,7 +9287,7 @@
       <c r="D266" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="E266" s="1">
+      <c r="E266" s="3">
         <v>12341234</v>
       </c>
       <c r="F266" s="2">
@@ -9301,7 +9313,7 @@
       <c r="D267" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="E267" s="1">
+      <c r="E267" s="3">
         <v>236154458446</v>
       </c>
       <c r="F267" s="1" t="s">
@@ -9327,7 +9339,7 @@
       <c r="D268" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="E268" s="1">
+      <c r="E268" s="3">
         <v>2355415596</v>
       </c>
       <c r="F268" s="1" t="s">
@@ -9353,7 +9365,7 @@
       <c r="D269" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E269" s="1">
+      <c r="E269" s="3">
         <v>43892236</v>
       </c>
       <c r="F269" s="1" t="s">
@@ -9379,7 +9391,7 @@
       <c r="D270" s="1" t="s">
         <v>471</v>
       </c>
-      <c r="E270" s="1">
+      <c r="E270" s="3">
         <v>42384156</v>
       </c>
       <c r="F270" s="1" t="s">
@@ -9405,7 +9417,7 @@
       <c r="D271" s="1" t="s">
         <v>473</v>
       </c>
-      <c r="E271" s="1">
+      <c r="E271" s="3">
         <v>1134509053</v>
       </c>
       <c r="F271" s="2">
@@ -9431,7 +9443,7 @@
       <c r="D272" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="E272" s="1">
+      <c r="E272" s="3">
         <v>1122881821</v>
       </c>
       <c r="F272" s="1" t="s">
@@ -9457,7 +9469,7 @@
       <c r="D273" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="E273" s="1">
+      <c r="E273" s="3">
         <v>42296000</v>
       </c>
       <c r="F273" s="1" t="s">
@@ -9483,7 +9495,7 @@
       <c r="D274" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="E274" s="1">
+      <c r="E274" s="3">
         <v>1134911674</v>
       </c>
       <c r="F274" s="1" t="s">
@@ -9509,7 +9521,7 @@
       <c r="D275" s="1" t="s">
         <v>481</v>
       </c>
-      <c r="E275" s="1">
+      <c r="E275" s="3">
         <v>1132602548</v>
       </c>
       <c r="F275" s="1" t="s">
@@ -9535,7 +9547,7 @@
       <c r="D276" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="E276" s="1">
+      <c r="E276" s="3">
         <v>1133340535</v>
       </c>
       <c r="F276" s="1" t="s">
@@ -9561,7 +9573,7 @@
       <c r="D277" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="E277" s="1">
+      <c r="E277" s="3">
         <v>1168754042</v>
       </c>
       <c r="F277" s="1" t="s">
@@ -9587,7 +9599,7 @@
       <c r="D278" s="1" t="s">
         <v>487</v>
       </c>
-      <c r="E278" s="1">
+      <c r="E278" s="3">
         <v>1131656801</v>
       </c>
       <c r="F278" s="1" t="s">
@@ -9613,7 +9625,7 @@
       <c r="D279" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="E279" s="1">
+      <c r="E279" s="3">
         <v>1126439830</v>
       </c>
       <c r="F279" s="1" t="s">
@@ -9639,7 +9651,7 @@
       <c r="D280" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="E280" s="1">
+      <c r="E280" s="3">
         <v>1167917116</v>
       </c>
       <c r="F280" s="1" t="s">
@@ -9665,7 +9677,7 @@
       <c r="D281" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="E281" s="1">
+      <c r="E281" s="3">
         <v>1136768700</v>
       </c>
       <c r="F281" s="1" t="s">
@@ -9691,7 +9703,7 @@
       <c r="D282" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="E282" s="1">
+      <c r="E282" s="3">
         <v>1130183974</v>
       </c>
       <c r="F282" s="1" t="s">
@@ -9717,7 +9729,7 @@
       <c r="D283" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E283" s="1">
+      <c r="E283" s="3">
         <v>11533993084</v>
       </c>
       <c r="F283" s="1" t="s">
@@ -9743,7 +9755,7 @@
       <c r="D284" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="E284" s="1">
+      <c r="E284" s="3">
         <v>57205244</v>
       </c>
       <c r="F284" s="1" t="s">
@@ -9769,7 +9781,7 @@
       <c r="D285" s="1" t="s">
         <v>578</v>
       </c>
-      <c r="E285" s="1">
+      <c r="E285" s="3">
         <v>1537728310</v>
       </c>
       <c r="F285" s="2">
@@ -9795,7 +9807,7 @@
       <c r="D286" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="E286" s="1">
+      <c r="E286" s="3">
         <v>58715897</v>
       </c>
       <c r="F286" s="1" t="s">
@@ -9821,7 +9833,7 @@
       <c r="D287" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="E287" s="1">
+      <c r="E287" s="3">
         <v>1139025242</v>
       </c>
       <c r="F287" s="1" t="s">
@@ -9847,7 +9859,7 @@
       <c r="D288" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="E288" s="1">
+      <c r="E288" s="3">
         <v>1154755467</v>
       </c>
       <c r="F288" s="1" t="s">
@@ -9873,7 +9885,7 @@
       <c r="D289" s="1" t="s">
         <v>506</v>
       </c>
-      <c r="E289" s="1">
+      <c r="E289" s="3">
         <v>1131749699</v>
       </c>
       <c r="F289" s="1" t="s">
@@ -9899,7 +9911,7 @@
       <c r="D290" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="E290" s="1">
+      <c r="E290" s="3">
         <v>1564725044</v>
       </c>
       <c r="F290" s="1" t="s">
@@ -9925,7 +9937,7 @@
       <c r="D291" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="E291" s="1">
+      <c r="E291" s="3">
         <v>40998725</v>
       </c>
       <c r="F291" s="1" t="s">
@@ -9951,7 +9963,7 @@
       <c r="D292" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="E292" s="1">
+      <c r="E292" s="3">
         <v>1534454303</v>
       </c>
       <c r="F292" s="1" t="s">
@@ -9977,7 +9989,7 @@
       <c r="D293" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="E293" s="1">
+      <c r="E293" s="3">
         <v>45818253</v>
       </c>
       <c r="F293" s="1" t="s">
@@ -10003,7 +10015,7 @@
       <c r="D294" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="E294" s="1">
+      <c r="E294" s="3">
         <v>2473472149</v>
       </c>
       <c r="F294" s="1" t="s">
@@ -10029,7 +10041,7 @@
       <c r="D295" s="1" t="s">
         <v>518</v>
       </c>
-      <c r="E295" s="1">
+      <c r="E295" s="3">
         <v>235569979</v>
       </c>
       <c r="F295" s="1" t="s">
@@ -10055,7 +10067,7 @@
       <c r="D296" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="E296" s="1">
+      <c r="E296" s="3">
         <v>236114260010</v>
       </c>
       <c r="F296" s="1" t="s">
@@ -10081,7 +10093,7 @@
       <c r="D297" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="E297" s="1">
+      <c r="E297" s="3">
         <v>236114260010</v>
       </c>
       <c r="F297" s="1" t="s">
@@ -10107,7 +10119,7 @@
       <c r="D298" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="E298" s="1">
+      <c r="E298" s="3">
         <v>45714121</v>
       </c>
       <c r="F298" s="2">
@@ -10133,7 +10145,7 @@
       <c r="D299" s="1" t="s">
         <v>583</v>
       </c>
-      <c r="E299" s="1">
+      <c r="E299" s="3">
         <v>40438816</v>
       </c>
       <c r="F299" s="1" t="s">
@@ -10159,7 +10171,7 @@
       <c r="D300" s="1" t="s">
         <v>585</v>
       </c>
-      <c r="E300" s="1">
+      <c r="E300" s="3">
         <v>42452952</v>
       </c>
       <c r="F300" s="2">
@@ -10185,7 +10197,7 @@
       <c r="D301" s="1" t="s">
         <v>587</v>
       </c>
-      <c r="E301" s="1">
+      <c r="E301" s="3">
         <v>1133423556</v>
       </c>
       <c r="F301" s="2">
@@ -10211,7 +10223,7 @@
       <c r="D302" s="1" t="s">
         <v>589</v>
       </c>
-      <c r="E302" s="1">
+      <c r="E302" s="3">
         <v>42946354</v>
       </c>
       <c r="F302" s="2">
@@ -10237,7 +10249,7 @@
       <c r="D303" s="1" t="s">
         <v>591</v>
       </c>
-      <c r="E303" s="1">
+      <c r="E303" s="3">
         <v>1137954376</v>
       </c>
       <c r="F303" s="2">
@@ -10263,7 +10275,7 @@
       <c r="D304" s="1" t="s">
         <v>593</v>
       </c>
-      <c r="E304" s="1">
+      <c r="E304" s="3">
         <v>1122030515</v>
       </c>
       <c r="F304" s="2">
@@ -10289,7 +10301,7 @@
       <c r="D305" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="E305" s="1">
+      <c r="E305" s="3">
         <v>1136933181</v>
       </c>
       <c r="F305" s="2">
@@ -10315,7 +10327,7 @@
       <c r="D306" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="E306" s="1">
+      <c r="E306" s="3">
         <v>45526974</v>
       </c>
       <c r="F306" s="2">
@@ -10341,7 +10353,7 @@
       <c r="D307" s="1" t="s">
         <v>599</v>
       </c>
-      <c r="E307" s="1">
+      <c r="E307" s="3">
         <v>46740443</v>
       </c>
       <c r="F307" s="2">
@@ -10367,7 +10379,7 @@
       <c r="D308" s="1" t="s">
         <v>601</v>
       </c>
-      <c r="E308" s="1">
+      <c r="E308" s="3">
         <v>1131550644</v>
       </c>
       <c r="F308" s="2">
@@ -10393,7 +10405,7 @@
       <c r="D309" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="E309" s="1">
+      <c r="E309" s="3">
         <v>1159423614</v>
       </c>
       <c r="F309" s="2">
@@ -10419,7 +10431,7 @@
       <c r="D310" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="E310" s="1">
+      <c r="E310" s="3">
         <v>65584451</v>
       </c>
       <c r="F310" s="2">
@@ -10445,7 +10457,7 @@
       <c r="D311" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="E311" s="1">
+      <c r="E311" s="3">
         <v>1545774297</v>
       </c>
       <c r="F311" s="2">
@@ -10471,7 +10483,7 @@
       <c r="D312" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="E312" s="1">
+      <c r="E312" s="3">
         <v>1132058180</v>
       </c>
       <c r="F312" s="2">
@@ -10497,7 +10509,7 @@
       <c r="D313" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="E313" s="1">
+      <c r="E313" s="3">
         <v>56470803</v>
       </c>
       <c r="F313" s="2">
@@ -10523,7 +10535,7 @@
       <c r="D314" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="E314" s="1">
+      <c r="E314" s="3">
         <v>1155967470</v>
       </c>
       <c r="F314" s="2">
@@ -10549,7 +10561,7 @@
       <c r="D315" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="E315" s="1">
+      <c r="E315" s="3">
         <v>1137332196</v>
       </c>
       <c r="F315" s="2">
@@ -10575,7 +10587,7 @@
       <c r="D316" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="E316" s="1">
+      <c r="E316" s="3">
         <v>1133848675</v>
       </c>
       <c r="F316" s="2">
@@ -10601,7 +10613,7 @@
       <c r="D317" s="1" t="s">
         <v>619</v>
       </c>
-      <c r="E317" s="1">
+      <c r="E317" s="3">
         <v>46353328</v>
       </c>
       <c r="F317" s="2">
@@ -10627,7 +10639,7 @@
       <c r="D318" s="1" t="s">
         <v>621</v>
       </c>
-      <c r="E318" s="1">
+      <c r="E318" s="3">
         <v>35945219</v>
       </c>
       <c r="F318" s="2">
@@ -10653,7 +10665,7 @@
       <c r="D319" s="1" t="s">
         <v>622</v>
       </c>
-      <c r="E319" s="1">
+      <c r="E319" s="3">
         <v>1566436850</v>
       </c>
       <c r="F319" s="2">
@@ -10679,7 +10691,7 @@
       <c r="D320" s="1" t="s">
         <v>624</v>
       </c>
-      <c r="E320" s="1">
+      <c r="E320" s="3">
         <v>1120565893</v>
       </c>
       <c r="F320" s="2">
@@ -10705,7 +10717,7 @@
       <c r="D321" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="E321" s="1">
+      <c r="E321" s="3">
         <v>40809000</v>
       </c>
       <c r="F321" s="2">
@@ -10731,7 +10743,7 @@
       <c r="D322" s="1" t="s">
         <v>628</v>
       </c>
-      <c r="E322" s="1">
+      <c r="E322" s="3">
         <v>2473410899</v>
       </c>
       <c r="F322" s="2">
@@ -10757,7 +10769,7 @@
       <c r="D323" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="E323" s="1">
+      <c r="E323" s="3">
         <v>236154505268</v>
       </c>
       <c r="F323" s="2">
@@ -10783,7 +10795,7 @@
       <c r="D324" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="E324" s="1">
+      <c r="E324" s="3">
         <v>2364548393</v>
       </c>
       <c r="F324" s="2">
@@ -10809,7 +10821,7 @@
       <c r="D325" s="1" t="s">
         <v>634</v>
       </c>
-      <c r="E325" s="1">
+      <c r="E325" s="3">
         <v>23358401129</v>
       </c>
       <c r="F325" s="2">
@@ -10835,7 +10847,7 @@
       <c r="D326" s="1" t="s">
         <v>636</v>
       </c>
-      <c r="E326" s="1">
+      <c r="E326" s="3">
         <v>1161725934</v>
       </c>
       <c r="F326" s="2">
@@ -10861,7 +10873,7 @@
       <c r="D327" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E327" s="1">
+      <c r="E327" s="3">
         <v>42646321</v>
       </c>
       <c r="F327" s="2">
@@ -10887,7 +10899,7 @@
       <c r="D328" s="1" t="s">
         <v>640</v>
       </c>
-      <c r="E328" s="1">
+      <c r="E328" s="3">
         <v>1558355329</v>
       </c>
       <c r="F328" s="2">
@@ -10913,7 +10925,7 @@
       <c r="D329" s="1" t="s">
         <v>642</v>
       </c>
-      <c r="E329" s="1">
+      <c r="E329" s="3">
         <v>36755390</v>
       </c>
       <c r="F329" s="2">
@@ -10939,7 +10951,7 @@
       <c r="D330" s="1" t="s">
         <v>644</v>
       </c>
-      <c r="E330" s="1">
+      <c r="E330" s="3">
         <v>45535941</v>
       </c>
       <c r="F330" s="2">
@@ -10965,7 +10977,7 @@
       <c r="D331" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="E331" s="1">
+      <c r="E331" s="3">
         <v>1151656256</v>
       </c>
       <c r="F331" s="2">
@@ -10991,7 +11003,7 @@
       <c r="D332" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="E332" s="1">
+      <c r="E332" s="3">
         <v>1562717491</v>
       </c>
       <c r="F332" s="2">
@@ -11017,7 +11029,7 @@
       <c r="D333" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="E333" s="1">
+      <c r="E333" s="3">
         <v>28987977</v>
       </c>
       <c r="F333" s="2">
@@ -11043,7 +11055,7 @@
       <c r="D334" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="E334" s="1">
+      <c r="E334" s="3">
         <v>1122978419</v>
       </c>
       <c r="F334" s="2">
@@ -11069,7 +11081,7 @@
       <c r="D335" s="1" t="s">
         <v>654</v>
       </c>
-      <c r="E335" s="1">
+      <c r="E335" s="3">
         <v>1165674003</v>
       </c>
       <c r="F335" s="2">
@@ -11095,7 +11107,7 @@
       <c r="D336" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="E336" s="1">
+      <c r="E336" s="3">
         <v>1163040420</v>
       </c>
       <c r="F336" s="2">
@@ -11106,6 +11118,58 @@
       </c>
       <c r="H336" s="3">
         <v>15040974450100</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A337" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C337" s="1">
+        <v>7846601</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="E337" s="3">
+        <v>112309520</v>
+      </c>
+      <c r="F337" s="2">
+        <v>11325</v>
+      </c>
+      <c r="G337" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H337" s="3">
+        <v>15067618020100</v>
+      </c>
+    </row>
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A338" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C338" s="1">
+        <v>6060076</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E338" s="3">
+        <v>1557307666</v>
+      </c>
+      <c r="F338" s="2">
+        <v>11325</v>
+      </c>
+      <c r="G338" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H338" s="3">
+        <v>15580532890800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>